<commit_message>
Adding additional dataset for MESH-CLASS
</commit_message>
<xml_diff>
--- a/data/Model_setups_GRIP.xlsx
+++ b/data/Model_setups_GRIP.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/j6mai/Documents/GitHub/Publications/mai_GRIP-E/tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/j6mai/Documents/GitHub/GRIP-E/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E91198A-6E57-7744-87A1-3E9B8E82E555}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41438857-5BF7-4C4C-9EB4-1E0D98D5B062}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28800" yWindow="-700" windowWidth="28420" windowHeight="16280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="223">
   <si>
     <t>MODEL</t>
   </si>
@@ -710,6 +710,9 @@
   </si>
   <si>
     <t>USGS (GTOPO 30, 1996; for surface/soil slope computation); HydroSHEDS 1km (for delineation and routing); NHN/NHD (vector; for drainage density)</t>
+  </si>
+  <si>
+    <t>1- Global Soil Dataset for Earth System Models (GSDE); https://agupubs.onlinelibrary.wiley.com/doi/full/10.1002/2013MS000293, 2- Global Depth to Bedrock Dataset for Earth System Modeling (250m)performing aggregation using QGIS (zonal stats as done for GSDE) (http://globalchange.bnu.edu.cn/research/dtb.jsp)</t>
   </si>
 </sst>
 </file>
@@ -1023,17 +1026,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1044,8 +1038,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1053,8 +1053,11 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="109">
@@ -1506,10 +1509,10 @@
   <dimension ref="A1:U140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="N9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R132" sqref="R132:U140"/>
+      <selection pane="bottomRight" activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1521,12 +1524,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
       <c r="E1" s="3" t="s">
         <v>199</v>
       </c>
@@ -1580,12 +1583,12 @@
       </c>
     </row>
     <row r="2" spans="1:21" ht="68" x14ac:dyDescent="0.2">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
       <c r="E2" s="25" t="s">
         <v>201</v>
       </c>
@@ -1639,12 +1642,12 @@
       </c>
     </row>
     <row r="3" spans="1:21" ht="51" x14ac:dyDescent="0.2">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
       <c r="E3" s="26" t="s">
         <v>189</v>
       </c>
@@ -1698,12 +1701,12 @@
       </c>
     </row>
     <row r="4" spans="1:21" ht="51" x14ac:dyDescent="0.2">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="25" t="s">
         <v>25</v>
       </c>
@@ -1757,12 +1760,12 @@
       </c>
     </row>
     <row r="5" spans="1:21" ht="85" x14ac:dyDescent="0.2">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
       <c r="E5" s="2" t="s">
         <v>207</v>
       </c>
@@ -1816,12 +1819,12 @@
       </c>
     </row>
     <row r="6" spans="1:21" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
       <c r="E6" s="25" t="s">
         <v>203</v>
       </c>
@@ -1875,14 +1878,14 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="102" x14ac:dyDescent="0.2">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
       <c r="E7" s="8" t="s">
         <v>53</v>
       </c>
@@ -1936,12 +1939,12 @@
       </c>
     </row>
     <row r="8" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="29"/>
-      <c r="B8" s="29" t="s">
+      <c r="A8" s="33"/>
+      <c r="B8" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
       <c r="E8" s="8" t="s">
         <v>54</v>
       </c>
@@ -1995,12 +1998,12 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="68" x14ac:dyDescent="0.2">
-      <c r="A9" s="29"/>
-      <c r="B9" s="29" t="s">
+      <c r="A9" s="33"/>
+      <c r="B9" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
       <c r="E9" s="26" t="s">
         <v>208</v>
       </c>
@@ -2046,30 +2049,30 @@
       <c r="U9" s="8"/>
     </row>
     <row r="10" spans="1:21" ht="255" x14ac:dyDescent="0.2">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="39" t="s">
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="29" t="s">
         <v>204</v>
       </c>
-      <c r="F10" s="39" t="s">
+      <c r="F10" s="29" t="s">
         <v>204</v>
       </c>
-      <c r="G10" s="39" t="s">
+      <c r="G10" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="39" t="s">
+      <c r="H10" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="I10" s="39" t="s">
+      <c r="I10" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="J10" s="39" t="s">
+      <c r="J10" s="29" t="s">
         <v>56</v>
       </c>
       <c r="K10" s="6" t="s">
@@ -2100,25 +2103,25 @@
         <v>170</v>
       </c>
       <c r="T10" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="U10" s="39" t="s">
+        <v>222</v>
+      </c>
+      <c r="U10" s="29" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="68" x14ac:dyDescent="0.2">
-      <c r="A11" s="30"/>
-      <c r="B11" s="30" t="s">
+      <c r="A11" s="38"/>
+      <c r="B11" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="39"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
       <c r="K11" s="6" t="s">
         <v>80</v>
       </c>
@@ -2149,21 +2152,21 @@
       <c r="T11" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="U11" s="39"/>
+      <c r="U11" s="29"/>
     </row>
     <row r="12" spans="1:21" ht="119" x14ac:dyDescent="0.2">
-      <c r="A12" s="30"/>
-      <c r="B12" s="30" t="s">
+      <c r="A12" s="38"/>
+      <c r="B12" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
       <c r="K12" s="10" t="s">
         <v>82</v>
       </c>
@@ -2194,33 +2197,33 @@
       <c r="T12" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="U12" s="39"/>
+      <c r="U12" s="29"/>
     </row>
     <row r="13" spans="1:21" ht="102" x14ac:dyDescent="0.2">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="35" t="s">
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="32" t="s">
         <v>205</v>
       </c>
-      <c r="F13" s="35" t="s">
+      <c r="F13" s="32" t="s">
         <v>205</v>
       </c>
-      <c r="G13" s="35" t="s">
+      <c r="G13" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="35" t="s">
+      <c r="H13" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="I13" s="35" t="s">
+      <c r="I13" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="J13" s="35" t="s">
+      <c r="J13" s="32" t="s">
         <v>67</v>
       </c>
       <c r="K13" s="2" t="s">
@@ -2258,18 +2261,18 @@
       </c>
     </row>
     <row r="14" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="29"/>
-      <c r="B14" s="29" t="s">
+      <c r="A14" s="33"/>
+      <c r="B14" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
       <c r="K14" s="8" t="s">
         <v>84</v>
       </c>
@@ -2305,18 +2308,18 @@
       </c>
     </row>
     <row r="15" spans="1:21" ht="136" x14ac:dyDescent="0.2">
-      <c r="A15" s="29"/>
-      <c r="B15" s="29" t="s">
+      <c r="A15" s="33"/>
+      <c r="B15" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="35"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
       <c r="K15" s="8"/>
       <c r="L15" s="8"/>
       <c r="M15" s="2" t="s">
@@ -2348,13 +2351,13 @@
       </c>
     </row>
     <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="36" t="s">
+      <c r="A16" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="32"/>
+      <c r="C16" s="35"/>
       <c r="D16" s="14" t="s">
         <v>14</v>
       </c>
@@ -2411,9 +2414,9 @@
       </c>
     </row>
     <row r="17" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="36"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
+      <c r="A17" s="34"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
       <c r="D17" s="14" t="s">
         <v>46</v>
       </c>
@@ -2470,9 +2473,9 @@
       </c>
     </row>
     <row r="18" spans="1:21" ht="68" x14ac:dyDescent="0.2">
-      <c r="A18" s="36"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
+      <c r="A18" s="34"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="35"/>
       <c r="D18" s="14" t="s">
         <v>43</v>
       </c>
@@ -2525,9 +2528,9 @@
       </c>
     </row>
     <row r="19" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="36"/>
-      <c r="B19" s="32"/>
-      <c r="C19" s="32"/>
+      <c r="A19" s="34"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
       <c r="D19" s="14" t="s">
         <v>45</v>
       </c>
@@ -2584,9 +2587,9 @@
       </c>
     </row>
     <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="36"/>
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
+      <c r="A20" s="34"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
       <c r="D20" s="14" t="s">
         <v>44</v>
       </c>
@@ -2643,11 +2646,11 @@
       </c>
     </row>
     <row r="21" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="36"/>
-      <c r="B21" s="37" t="s">
+      <c r="A21" s="34"/>
+      <c r="B21" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="37"/>
+      <c r="C21" s="36"/>
       <c r="D21" s="16" t="s">
         <v>14</v>
       </c>
@@ -2704,9 +2707,9 @@
       </c>
     </row>
     <row r="22" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="36"/>
-      <c r="B22" s="37"/>
-      <c r="C22" s="37"/>
+      <c r="A22" s="34"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="36"/>
       <c r="D22" s="16" t="s">
         <v>46</v>
       </c>
@@ -2763,9 +2766,9 @@
       </c>
     </row>
     <row r="23" spans="1:21" ht="68" x14ac:dyDescent="0.2">
-      <c r="A23" s="36"/>
-      <c r="B23" s="37"/>
-      <c r="C23" s="37"/>
+      <c r="A23" s="34"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
       <c r="D23" s="16" t="s">
         <v>43</v>
       </c>
@@ -2818,9 +2821,9 @@
       </c>
     </row>
     <row r="24" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="36"/>
-      <c r="B24" s="37"/>
-      <c r="C24" s="37"/>
+      <c r="A24" s="34"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="36"/>
       <c r="D24" s="16" t="s">
         <v>45</v>
       </c>
@@ -2877,9 +2880,9 @@
       </c>
     </row>
     <row r="25" spans="1:21" ht="32" x14ac:dyDescent="0.2">
-      <c r="A25" s="36"/>
-      <c r="B25" s="37"/>
-      <c r="C25" s="37"/>
+      <c r="A25" s="34"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="36"/>
       <c r="D25" s="16" t="s">
         <v>44</v>
       </c>
@@ -2936,30 +2939,30 @@
       </c>
     </row>
     <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="36"/>
-      <c r="B26" s="32" t="s">
+      <c r="A26" s="34"/>
+      <c r="B26" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="32"/>
+      <c r="C26" s="35"/>
       <c r="D26" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E26" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="F26" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="G26" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="H26" s="39" t="s">
+      <c r="E26" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="F26" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G26" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="H26" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="I26" s="39" t="s">
+      <c r="I26" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="J26" s="34" t="s">
+      <c r="J26" s="31" t="s">
         <v>42</v>
       </c>
       <c r="K26" s="6" t="s">
@@ -2968,13 +2971,13 @@
       <c r="L26" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="M26" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="N26" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="O26" s="34" t="s">
+      <c r="M26" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="N26" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="O26" s="31" t="s">
         <v>42</v>
       </c>
       <c r="P26" s="6" t="s">
@@ -2992,32 +2995,32 @@
       <c r="T26" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="U26" s="39" t="s">
+      <c r="U26" s="29" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="36"/>
-      <c r="B27" s="32"/>
-      <c r="C27" s="32"/>
+      <c r="A27" s="34"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="35"/>
       <c r="D27" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="39"/>
-      <c r="I27" s="39"/>
-      <c r="J27" s="34"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="31"/>
       <c r="K27" s="2" t="s">
         <v>34</v>
       </c>
       <c r="L27" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="M27" s="39"/>
-      <c r="N27" s="39"/>
-      <c r="O27" s="34"/>
+      <c r="M27" s="29"/>
+      <c r="N27" s="29"/>
+      <c r="O27" s="31"/>
       <c r="P27" s="10" t="s">
         <v>58</v>
       </c>
@@ -3033,30 +3036,30 @@
       <c r="T27" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="U27" s="39"/>
+      <c r="U27" s="29"/>
     </row>
     <row r="28" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="36"/>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
+      <c r="A28" s="34"/>
+      <c r="B28" s="35"/>
+      <c r="C28" s="35"/>
       <c r="D28" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="34"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="31"/>
       <c r="K28" s="5" t="s">
         <v>89</v>
       </c>
       <c r="L28" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="M28" s="39"/>
-      <c r="N28" s="39"/>
-      <c r="O28" s="34"/>
+      <c r="M28" s="29"/>
+      <c r="N28" s="29"/>
+      <c r="O28" s="31"/>
       <c r="P28" s="10" t="s">
         <v>59</v>
       </c>
@@ -3072,30 +3075,30 @@
       <c r="T28" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="U28" s="39"/>
+      <c r="U28" s="29"/>
     </row>
     <row r="29" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="36"/>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
+      <c r="A29" s="34"/>
+      <c r="B29" s="35"/>
+      <c r="C29" s="35"/>
       <c r="D29" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E29" s="34"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="34"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="34"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="31"/>
       <c r="K29" s="5" t="s">
         <v>90</v>
       </c>
       <c r="L29" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="M29" s="39"/>
-      <c r="N29" s="39"/>
-      <c r="O29" s="34"/>
+      <c r="M29" s="29"/>
+      <c r="N29" s="29"/>
+      <c r="O29" s="31"/>
       <c r="P29" s="6" t="s">
         <v>147</v>
       </c>
@@ -3111,30 +3114,30 @@
       <c r="T29" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="U29" s="39"/>
+      <c r="U29" s="29"/>
     </row>
     <row r="30" spans="1:21" ht="32" x14ac:dyDescent="0.2">
-      <c r="A30" s="36"/>
-      <c r="B30" s="32"/>
-      <c r="C30" s="32"/>
+      <c r="A30" s="34"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="35"/>
       <c r="D30" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="34"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="39"/>
-      <c r="J30" s="34"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="31"/>
       <c r="K30" s="5" t="s">
         <v>91</v>
       </c>
       <c r="L30" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="M30" s="39"/>
-      <c r="N30" s="39"/>
-      <c r="O30" s="34"/>
+      <c r="M30" s="29"/>
+      <c r="N30" s="29"/>
+      <c r="O30" s="31"/>
       <c r="P30" s="5" t="s">
         <v>37</v>
       </c>
@@ -3150,48 +3153,48 @@
       <c r="T30" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="U30" s="39"/>
+      <c r="U30" s="29"/>
     </row>
     <row r="31" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="36"/>
-      <c r="B31" s="37" t="s">
+      <c r="A31" s="34"/>
+      <c r="B31" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="37"/>
+      <c r="C31" s="36"/>
       <c r="D31" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E31" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="F31" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="G31" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="H31" s="33" t="s">
+      <c r="E31" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="F31" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="G31" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="H31" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="I31" s="33" t="s">
+      <c r="I31" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="J31" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="K31" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="L31" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="M31" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="N31" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="O31" s="33" t="s">
+      <c r="J31" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="K31" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="L31" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="M31" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="N31" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="O31" s="30" t="s">
         <v>42</v>
       </c>
       <c r="P31" s="8" t="s">
@@ -3209,28 +3212,28 @@
       <c r="T31" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="U31" s="33" t="s">
+      <c r="U31" s="30" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="36"/>
-      <c r="B32" s="37"/>
-      <c r="C32" s="37"/>
+      <c r="A32" s="34"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
       <c r="D32" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="E32" s="33"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="33"/>
-      <c r="H32" s="33"/>
-      <c r="I32" s="33"/>
-      <c r="J32" s="35"/>
-      <c r="K32" s="35"/>
-      <c r="L32" s="35"/>
-      <c r="M32" s="35"/>
-      <c r="N32" s="35"/>
-      <c r="O32" s="33"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="30"/>
+      <c r="I32" s="30"/>
+      <c r="J32" s="32"/>
+      <c r="K32" s="32"/>
+      <c r="L32" s="32"/>
+      <c r="M32" s="32"/>
+      <c r="N32" s="32"/>
+      <c r="O32" s="30"/>
       <c r="P32" s="8" t="s">
         <v>87</v>
       </c>
@@ -3246,26 +3249,26 @@
       <c r="T32" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="U32" s="33"/>
+      <c r="U32" s="30"/>
     </row>
     <row r="33" spans="1:21" ht="32" x14ac:dyDescent="0.2">
-      <c r="A33" s="36"/>
-      <c r="B33" s="37"/>
-      <c r="C33" s="37"/>
+      <c r="A33" s="34"/>
+      <c r="B33" s="36"/>
+      <c r="C33" s="36"/>
       <c r="D33" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="E33" s="33"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="33"/>
-      <c r="H33" s="33"/>
-      <c r="I33" s="33"/>
-      <c r="J33" s="35"/>
-      <c r="K33" s="35"/>
-      <c r="L33" s="35"/>
-      <c r="M33" s="35"/>
-      <c r="N33" s="35"/>
-      <c r="O33" s="33"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="32"/>
+      <c r="K33" s="32"/>
+      <c r="L33" s="32"/>
+      <c r="M33" s="32"/>
+      <c r="N33" s="32"/>
+      <c r="O33" s="30"/>
       <c r="P33" s="8" t="s">
         <v>59</v>
       </c>
@@ -3281,26 +3284,26 @@
       <c r="T33" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="U33" s="33"/>
+      <c r="U33" s="30"/>
     </row>
     <row r="34" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="36"/>
-      <c r="B34" s="37"/>
-      <c r="C34" s="37"/>
+      <c r="A34" s="34"/>
+      <c r="B34" s="36"/>
+      <c r="C34" s="36"/>
       <c r="D34" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="E34" s="33"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="33"/>
-      <c r="H34" s="33"/>
-      <c r="I34" s="33"/>
-      <c r="J34" s="35"/>
-      <c r="K34" s="35"/>
-      <c r="L34" s="35"/>
-      <c r="M34" s="35"/>
-      <c r="N34" s="35"/>
-      <c r="O34" s="33"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="30"/>
+      <c r="I34" s="30"/>
+      <c r="J34" s="32"/>
+      <c r="K34" s="32"/>
+      <c r="L34" s="32"/>
+      <c r="M34" s="32"/>
+      <c r="N34" s="32"/>
+      <c r="O34" s="30"/>
       <c r="P34" s="8" t="s">
         <v>147</v>
       </c>
@@ -3316,26 +3319,26 @@
       <c r="T34" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="U34" s="33"/>
+      <c r="U34" s="30"/>
     </row>
     <row r="35" spans="1:21" ht="32" x14ac:dyDescent="0.2">
-      <c r="A35" s="36"/>
-      <c r="B35" s="37"/>
-      <c r="C35" s="37"/>
+      <c r="A35" s="34"/>
+      <c r="B35" s="36"/>
+      <c r="C35" s="36"/>
       <c r="D35" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="E35" s="33"/>
-      <c r="F35" s="33"/>
-      <c r="G35" s="33"/>
-      <c r="H35" s="33"/>
-      <c r="I35" s="33"/>
-      <c r="J35" s="35"/>
-      <c r="K35" s="35"/>
-      <c r="L35" s="35"/>
-      <c r="M35" s="35"/>
-      <c r="N35" s="35"/>
-      <c r="O35" s="33"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="30"/>
+      <c r="I35" s="30"/>
+      <c r="J35" s="32"/>
+      <c r="K35" s="32"/>
+      <c r="L35" s="32"/>
+      <c r="M35" s="32"/>
+      <c r="N35" s="32"/>
+      <c r="O35" s="30"/>
       <c r="P35" s="8" t="s">
         <v>37</v>
       </c>
@@ -3351,48 +3354,48 @@
       <c r="T35" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="U35" s="33"/>
+      <c r="U35" s="30"/>
     </row>
     <row r="36" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="36"/>
-      <c r="B36" s="32" t="s">
+      <c r="A36" s="34"/>
+      <c r="B36" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="32"/>
+      <c r="C36" s="35"/>
       <c r="D36" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E36" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="F36" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="G36" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="H36" s="34" t="s">
+      <c r="E36" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="F36" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G36" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="H36" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="I36" s="34" t="s">
+      <c r="I36" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="J36" s="34" t="s">
+      <c r="J36" s="31" t="s">
         <v>42</v>
       </c>
       <c r="K36" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="L36" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="M36" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="N36" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="O36" s="34" t="s">
+      <c r="L36" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="M36" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="N36" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="O36" s="31" t="s">
         <v>42</v>
       </c>
       <c r="P36" s="6" t="s">
@@ -3410,30 +3413,30 @@
       <c r="T36" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="U36" s="39" t="s">
+      <c r="U36" s="29" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="36"/>
-      <c r="B37" s="32"/>
-      <c r="C37" s="32"/>
+      <c r="A37" s="34"/>
+      <c r="B37" s="35"/>
+      <c r="C37" s="35"/>
       <c r="D37" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
-      <c r="G37" s="34"/>
-      <c r="H37" s="34"/>
-      <c r="I37" s="34"/>
-      <c r="J37" s="34"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="31"/>
+      <c r="H37" s="31"/>
+      <c r="I37" s="31"/>
+      <c r="J37" s="31"/>
       <c r="K37" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="L37" s="34"/>
-      <c r="M37" s="39"/>
-      <c r="N37" s="39"/>
-      <c r="O37" s="34"/>
+      <c r="L37" s="31"/>
+      <c r="M37" s="29"/>
+      <c r="N37" s="29"/>
+      <c r="O37" s="31"/>
       <c r="P37" s="10" t="s">
         <v>87</v>
       </c>
@@ -3449,26 +3452,26 @@
       <c r="T37" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="U37" s="39"/>
+      <c r="U37" s="29"/>
     </row>
     <row r="38" spans="1:21" ht="34" x14ac:dyDescent="0.2">
-      <c r="A38" s="36"/>
-      <c r="B38" s="32"/>
-      <c r="C38" s="32"/>
+      <c r="A38" s="34"/>
+      <c r="B38" s="35"/>
+      <c r="C38" s="35"/>
       <c r="D38" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="E38" s="34"/>
-      <c r="F38" s="34"/>
-      <c r="G38" s="34"/>
-      <c r="H38" s="34"/>
-      <c r="I38" s="34"/>
-      <c r="J38" s="34"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="31"/>
+      <c r="H38" s="31"/>
+      <c r="I38" s="31"/>
+      <c r="J38" s="31"/>
       <c r="K38" s="5"/>
-      <c r="L38" s="34"/>
-      <c r="M38" s="39"/>
-      <c r="N38" s="39"/>
-      <c r="O38" s="34"/>
+      <c r="L38" s="31"/>
+      <c r="M38" s="29"/>
+      <c r="N38" s="29"/>
+      <c r="O38" s="31"/>
       <c r="P38" s="10" t="s">
         <v>59</v>
       </c>
@@ -3484,28 +3487,28 @@
       <c r="T38" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="U38" s="39"/>
+      <c r="U38" s="29"/>
     </row>
     <row r="39" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="36"/>
-      <c r="B39" s="32"/>
-      <c r="C39" s="32"/>
+      <c r="A39" s="34"/>
+      <c r="B39" s="35"/>
+      <c r="C39" s="35"/>
       <c r="D39" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E39" s="34"/>
-      <c r="F39" s="34"/>
-      <c r="G39" s="34"/>
-      <c r="H39" s="34"/>
-      <c r="I39" s="34"/>
-      <c r="J39" s="34"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="31"/>
+      <c r="H39" s="31"/>
+      <c r="I39" s="31"/>
+      <c r="J39" s="31"/>
       <c r="K39" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="L39" s="34"/>
-      <c r="M39" s="39"/>
-      <c r="N39" s="39"/>
-      <c r="O39" s="34"/>
+      <c r="L39" s="31"/>
+      <c r="M39" s="29"/>
+      <c r="N39" s="29"/>
+      <c r="O39" s="31"/>
       <c r="P39" s="5" t="s">
         <v>148</v>
       </c>
@@ -3521,28 +3524,28 @@
       <c r="T39" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="U39" s="39"/>
+      <c r="U39" s="29"/>
     </row>
     <row r="40" spans="1:21" ht="32" x14ac:dyDescent="0.2">
-      <c r="A40" s="36"/>
-      <c r="B40" s="32"/>
-      <c r="C40" s="32"/>
+      <c r="A40" s="34"/>
+      <c r="B40" s="35"/>
+      <c r="C40" s="35"/>
       <c r="D40" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="E40" s="34"/>
-      <c r="F40" s="34"/>
-      <c r="G40" s="34"/>
-      <c r="H40" s="34"/>
-      <c r="I40" s="34"/>
-      <c r="J40" s="34"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="31"/>
+      <c r="G40" s="31"/>
+      <c r="H40" s="31"/>
+      <c r="I40" s="31"/>
+      <c r="J40" s="31"/>
       <c r="K40" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="L40" s="34"/>
-      <c r="M40" s="39"/>
-      <c r="N40" s="39"/>
-      <c r="O40" s="34"/>
+      <c r="L40" s="31"/>
+      <c r="M40" s="29"/>
+      <c r="N40" s="29"/>
+      <c r="O40" s="31"/>
       <c r="P40" s="5" t="s">
         <v>149</v>
       </c>
@@ -3558,33 +3561,33 @@
       <c r="T40" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="U40" s="39"/>
+      <c r="U40" s="29"/>
     </row>
     <row r="41" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="36"/>
-      <c r="B41" s="37" t="s">
+      <c r="A41" s="34"/>
+      <c r="B41" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C41" s="37"/>
+      <c r="C41" s="36"/>
       <c r="D41" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E41" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="F41" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="G41" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="H41" s="35" t="s">
+      <c r="E41" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="F41" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="G41" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="H41" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="I41" s="35" t="s">
+      <c r="I41" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="J41" s="33" t="s">
+      <c r="J41" s="30" t="s">
         <v>42</v>
       </c>
       <c r="K41" s="2" t="s">
@@ -3593,13 +3596,13 @@
       <c r="L41" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="M41" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="N41" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="O41" s="33" t="s">
+      <c r="M41" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="N41" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="O41" s="30" t="s">
         <v>42</v>
       </c>
       <c r="P41" s="8" t="s">
@@ -3617,32 +3620,32 @@
       <c r="T41" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="U41" s="33" t="s">
+      <c r="U41" s="30" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="42" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="36"/>
-      <c r="B42" s="37"/>
-      <c r="C42" s="37"/>
+      <c r="A42" s="34"/>
+      <c r="B42" s="36"/>
+      <c r="C42" s="36"/>
       <c r="D42" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="E42" s="33"/>
-      <c r="F42" s="33"/>
-      <c r="G42" s="33"/>
-      <c r="H42" s="35"/>
-      <c r="I42" s="35"/>
-      <c r="J42" s="33"/>
+      <c r="E42" s="30"/>
+      <c r="F42" s="30"/>
+      <c r="G42" s="30"/>
+      <c r="H42" s="32"/>
+      <c r="I42" s="32"/>
+      <c r="J42" s="30"/>
       <c r="K42" s="2" t="s">
         <v>34</v>
       </c>
       <c r="L42" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="M42" s="35"/>
-      <c r="N42" s="35"/>
-      <c r="O42" s="33"/>
+      <c r="M42" s="32"/>
+      <c r="N42" s="32"/>
+      <c r="O42" s="30"/>
       <c r="P42" s="8" t="s">
         <v>87</v>
       </c>
@@ -3658,30 +3661,30 @@
       <c r="T42" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="U42" s="33"/>
+      <c r="U42" s="30"/>
     </row>
     <row r="43" spans="1:21" ht="48" x14ac:dyDescent="0.2">
-      <c r="A43" s="36"/>
-      <c r="B43" s="37"/>
-      <c r="C43" s="37"/>
+      <c r="A43" s="34"/>
+      <c r="B43" s="36"/>
+      <c r="C43" s="36"/>
       <c r="D43" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="E43" s="33"/>
-      <c r="F43" s="33"/>
-      <c r="G43" s="33"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="33"/>
+      <c r="E43" s="30"/>
+      <c r="F43" s="30"/>
+      <c r="G43" s="30"/>
+      <c r="H43" s="32"/>
+      <c r="I43" s="32"/>
+      <c r="J43" s="30"/>
       <c r="K43" s="18" t="s">
         <v>94</v>
       </c>
       <c r="L43" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="M43" s="35"/>
-      <c r="N43" s="35"/>
-      <c r="O43" s="33"/>
+      <c r="M43" s="32"/>
+      <c r="N43" s="32"/>
+      <c r="O43" s="30"/>
       <c r="P43" s="8" t="s">
         <v>150</v>
       </c>
@@ -3697,30 +3700,30 @@
       <c r="T43" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="U43" s="33"/>
+      <c r="U43" s="30"/>
     </row>
     <row r="44" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="36"/>
-      <c r="B44" s="37"/>
-      <c r="C44" s="37"/>
+      <c r="A44" s="34"/>
+      <c r="B44" s="36"/>
+      <c r="C44" s="36"/>
       <c r="D44" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="E44" s="33"/>
-      <c r="F44" s="33"/>
-      <c r="G44" s="33"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="33"/>
+      <c r="E44" s="30"/>
+      <c r="F44" s="30"/>
+      <c r="G44" s="30"/>
+      <c r="H44" s="32"/>
+      <c r="I44" s="32"/>
+      <c r="J44" s="30"/>
       <c r="K44" s="2" t="s">
         <v>95</v>
       </c>
       <c r="L44" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="M44" s="35"/>
-      <c r="N44" s="35"/>
-      <c r="O44" s="33"/>
+      <c r="M44" s="32"/>
+      <c r="N44" s="32"/>
+      <c r="O44" s="30"/>
       <c r="P44" s="8" t="s">
         <v>148</v>
       </c>
@@ -3736,30 +3739,30 @@
       <c r="T44" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="U44" s="33"/>
+      <c r="U44" s="30"/>
     </row>
     <row r="45" spans="1:21" ht="68" x14ac:dyDescent="0.2">
-      <c r="A45" s="36"/>
-      <c r="B45" s="37"/>
-      <c r="C45" s="37"/>
+      <c r="A45" s="34"/>
+      <c r="B45" s="36"/>
+      <c r="C45" s="36"/>
       <c r="D45" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="E45" s="33"/>
-      <c r="F45" s="33"/>
-      <c r="G45" s="33"/>
-      <c r="H45" s="35"/>
-      <c r="I45" s="35"/>
-      <c r="J45" s="33"/>
+      <c r="E45" s="30"/>
+      <c r="F45" s="30"/>
+      <c r="G45" s="30"/>
+      <c r="H45" s="32"/>
+      <c r="I45" s="32"/>
+      <c r="J45" s="30"/>
       <c r="K45" s="2" t="s">
         <v>96</v>
       </c>
       <c r="L45" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="M45" s="35"/>
-      <c r="N45" s="35"/>
-      <c r="O45" s="33"/>
+      <c r="M45" s="32"/>
+      <c r="N45" s="32"/>
+      <c r="O45" s="30"/>
       <c r="P45" s="8" t="s">
         <v>151</v>
       </c>
@@ -3775,33 +3778,33 @@
       <c r="T45" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="U45" s="33"/>
+      <c r="U45" s="30"/>
     </row>
     <row r="46" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" s="36"/>
-      <c r="B46" s="32" t="s">
+      <c r="A46" s="34"/>
+      <c r="B46" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C46" s="32"/>
+      <c r="C46" s="35"/>
       <c r="D46" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E46" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="F46" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="G46" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="H46" s="38" t="s">
+      <c r="E46" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="F46" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G46" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="H46" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="I46" s="38" t="s">
+      <c r="I46" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="J46" s="34" t="s">
+      <c r="J46" s="31" t="s">
         <v>42</v>
       </c>
       <c r="K46" s="11" t="s">
@@ -3810,13 +3813,13 @@
       <c r="L46" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="M46" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="N46" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="O46" s="34" t="s">
+      <c r="M46" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="N46" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="O46" s="31" t="s">
         <v>42</v>
       </c>
       <c r="P46" s="10" t="s">
@@ -3825,7 +3828,7 @@
       <c r="Q46" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="R46" s="39" t="s">
+      <c r="R46" s="29" t="s">
         <v>42</v>
       </c>
       <c r="S46" s="6" t="s">
@@ -3834,326 +3837,326 @@
       <c r="T46" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="U46" s="39" t="s">
+      <c r="U46" s="29" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" s="36"/>
-      <c r="B47" s="32"/>
-      <c r="C47" s="32"/>
+      <c r="A47" s="34"/>
+      <c r="B47" s="35"/>
+      <c r="C47" s="35"/>
       <c r="D47" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="E47" s="34"/>
-      <c r="F47" s="34"/>
-      <c r="G47" s="34"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="38"/>
-      <c r="J47" s="34"/>
+      <c r="E47" s="31"/>
+      <c r="F47" s="31"/>
+      <c r="G47" s="31"/>
+      <c r="H47" s="37"/>
+      <c r="I47" s="37"/>
+      <c r="J47" s="31"/>
       <c r="K47" s="11" t="s">
         <v>34</v>
       </c>
       <c r="L47" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="M47" s="39"/>
-      <c r="N47" s="39"/>
-      <c r="O47" s="34"/>
+      <c r="M47" s="29"/>
+      <c r="N47" s="29"/>
+      <c r="O47" s="31"/>
       <c r="P47" s="10" t="s">
         <v>58</v>
       </c>
       <c r="Q47" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="R47" s="39"/>
+      <c r="R47" s="29"/>
       <c r="S47" s="6" t="s">
         <v>174</v>
       </c>
       <c r="T47" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="U47" s="39"/>
+      <c r="U47" s="29"/>
     </row>
     <row r="48" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="36"/>
-      <c r="B48" s="32"/>
-      <c r="C48" s="32"/>
+      <c r="A48" s="34"/>
+      <c r="B48" s="35"/>
+      <c r="C48" s="35"/>
       <c r="D48" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="E48" s="34"/>
-      <c r="F48" s="34"/>
-      <c r="G48" s="34"/>
-      <c r="H48" s="38"/>
-      <c r="I48" s="38"/>
-      <c r="J48" s="34"/>
+      <c r="E48" s="31"/>
+      <c r="F48" s="31"/>
+      <c r="G48" s="31"/>
+      <c r="H48" s="37"/>
+      <c r="I48" s="37"/>
+      <c r="J48" s="31"/>
       <c r="K48" s="11" t="s">
         <v>98</v>
       </c>
       <c r="L48" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="M48" s="39"/>
-      <c r="N48" s="39"/>
-      <c r="O48" s="34"/>
+      <c r="M48" s="29"/>
+      <c r="N48" s="29"/>
+      <c r="O48" s="31"/>
       <c r="P48" s="10" t="s">
         <v>152</v>
       </c>
       <c r="Q48" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="R48" s="39"/>
+      <c r="R48" s="29"/>
       <c r="S48" s="6" t="s">
         <v>196</v>
       </c>
       <c r="T48" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="U48" s="39"/>
+      <c r="U48" s="29"/>
     </row>
     <row r="49" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="A49" s="36"/>
-      <c r="B49" s="32"/>
-      <c r="C49" s="32"/>
+      <c r="A49" s="34"/>
+      <c r="B49" s="35"/>
+      <c r="C49" s="35"/>
       <c r="D49" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E49" s="34"/>
-      <c r="F49" s="34"/>
-      <c r="G49" s="34"/>
-      <c r="H49" s="38"/>
-      <c r="I49" s="38"/>
-      <c r="J49" s="34"/>
+      <c r="E49" s="31"/>
+      <c r="F49" s="31"/>
+      <c r="G49" s="31"/>
+      <c r="H49" s="37"/>
+      <c r="I49" s="37"/>
+      <c r="J49" s="31"/>
       <c r="K49" s="11" t="s">
         <v>99</v>
       </c>
       <c r="L49" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="M49" s="39"/>
-      <c r="N49" s="39"/>
-      <c r="O49" s="34"/>
+      <c r="M49" s="29"/>
+      <c r="N49" s="29"/>
+      <c r="O49" s="31"/>
       <c r="P49" s="6" t="s">
         <v>153</v>
       </c>
       <c r="Q49" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="R49" s="39"/>
+      <c r="R49" s="29"/>
       <c r="S49" s="6" t="s">
         <v>153</v>
       </c>
       <c r="T49" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="U49" s="39"/>
+      <c r="U49" s="29"/>
     </row>
     <row r="50" spans="1:21" ht="32" x14ac:dyDescent="0.2">
-      <c r="A50" s="36"/>
-      <c r="B50" s="32"/>
-      <c r="C50" s="32"/>
+      <c r="A50" s="34"/>
+      <c r="B50" s="35"/>
+      <c r="C50" s="35"/>
       <c r="D50" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="E50" s="34"/>
-      <c r="F50" s="34"/>
-      <c r="G50" s="34"/>
-      <c r="H50" s="38"/>
-      <c r="I50" s="38"/>
-      <c r="J50" s="34"/>
+      <c r="E50" s="31"/>
+      <c r="F50" s="31"/>
+      <c r="G50" s="31"/>
+      <c r="H50" s="37"/>
+      <c r="I50" s="37"/>
+      <c r="J50" s="31"/>
       <c r="K50" s="11" t="s">
         <v>100</v>
       </c>
       <c r="L50" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="M50" s="39"/>
-      <c r="N50" s="39"/>
-      <c r="O50" s="34"/>
+      <c r="M50" s="29"/>
+      <c r="N50" s="29"/>
+      <c r="O50" s="31"/>
       <c r="P50" s="6" t="s">
         <v>154</v>
       </c>
       <c r="Q50" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="R50" s="39"/>
+      <c r="R50" s="29"/>
       <c r="S50" s="6" t="s">
         <v>154</v>
       </c>
       <c r="T50" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="U50" s="39"/>
+      <c r="U50" s="29"/>
     </row>
     <row r="51" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="36"/>
-      <c r="B51" s="32" t="s">
+      <c r="A51" s="34"/>
+      <c r="B51" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="C51" s="32"/>
+      <c r="C51" s="35"/>
       <c r="D51" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E51" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="F51" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="G51" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="H51" s="34" t="s">
+      <c r="E51" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="F51" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G51" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="H51" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="I51" s="34" t="s">
+      <c r="I51" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="J51" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="K51" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="L51" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="M51" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="N51" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="O51" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="P51" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q51" s="39" t="s">
+      <c r="J51" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="K51" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="L51" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="M51" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="N51" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="O51" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="P51" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q51" s="29" t="s">
         <v>42</v>
       </c>
       <c r="R51" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="S51" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="T51" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="U51" s="39" t="s">
+      <c r="S51" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="T51" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="U51" s="29" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="52" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="A52" s="36"/>
-      <c r="B52" s="32"/>
-      <c r="C52" s="32"/>
+      <c r="A52" s="34"/>
+      <c r="B52" s="35"/>
+      <c r="C52" s="35"/>
       <c r="D52" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="E52" s="34"/>
-      <c r="F52" s="34"/>
-      <c r="G52" s="34"/>
-      <c r="H52" s="34"/>
-      <c r="I52" s="34"/>
-      <c r="J52" s="34"/>
-      <c r="K52" s="34"/>
-      <c r="L52" s="34"/>
-      <c r="M52" s="39"/>
-      <c r="N52" s="39"/>
-      <c r="O52" s="34"/>
-      <c r="P52" s="39"/>
-      <c r="Q52" s="39"/>
+      <c r="E52" s="31"/>
+      <c r="F52" s="31"/>
+      <c r="G52" s="31"/>
+      <c r="H52" s="31"/>
+      <c r="I52" s="31"/>
+      <c r="J52" s="31"/>
+      <c r="K52" s="31"/>
+      <c r="L52" s="31"/>
+      <c r="M52" s="29"/>
+      <c r="N52" s="29"/>
+      <c r="O52" s="31"/>
+      <c r="P52" s="29"/>
+      <c r="Q52" s="29"/>
       <c r="R52" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="S52" s="39"/>
-      <c r="T52" s="39"/>
-      <c r="U52" s="39"/>
+      <c r="S52" s="29"/>
+      <c r="T52" s="29"/>
+      <c r="U52" s="29"/>
     </row>
     <row r="53" spans="1:21" ht="34" x14ac:dyDescent="0.2">
-      <c r="A53" s="36"/>
-      <c r="B53" s="32"/>
-      <c r="C53" s="32"/>
+      <c r="A53" s="34"/>
+      <c r="B53" s="35"/>
+      <c r="C53" s="35"/>
       <c r="D53" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="E53" s="34"/>
-      <c r="F53" s="34"/>
-      <c r="G53" s="34"/>
-      <c r="H53" s="34"/>
-      <c r="I53" s="34"/>
-      <c r="J53" s="34"/>
-      <c r="K53" s="34"/>
-      <c r="L53" s="34"/>
-      <c r="M53" s="39"/>
-      <c r="N53" s="39"/>
-      <c r="O53" s="34"/>
-      <c r="P53" s="39"/>
-      <c r="Q53" s="39"/>
+      <c r="E53" s="31"/>
+      <c r="F53" s="31"/>
+      <c r="G53" s="31"/>
+      <c r="H53" s="31"/>
+      <c r="I53" s="31"/>
+      <c r="J53" s="31"/>
+      <c r="K53" s="31"/>
+      <c r="L53" s="31"/>
+      <c r="M53" s="29"/>
+      <c r="N53" s="29"/>
+      <c r="O53" s="31"/>
+      <c r="P53" s="29"/>
+      <c r="Q53" s="29"/>
       <c r="R53" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="S53" s="39"/>
-      <c r="T53" s="39"/>
-      <c r="U53" s="39"/>
+      <c r="S53" s="29"/>
+      <c r="T53" s="29"/>
+      <c r="U53" s="29"/>
     </row>
     <row r="54" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="A54" s="36"/>
-      <c r="B54" s="32"/>
-      <c r="C54" s="32"/>
+      <c r="A54" s="34"/>
+      <c r="B54" s="35"/>
+      <c r="C54" s="35"/>
       <c r="D54" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E54" s="34"/>
-      <c r="F54" s="34"/>
-      <c r="G54" s="34"/>
-      <c r="H54" s="34"/>
-      <c r="I54" s="34"/>
-      <c r="J54" s="34"/>
-      <c r="K54" s="34"/>
-      <c r="L54" s="34"/>
-      <c r="M54" s="39"/>
-      <c r="N54" s="39"/>
-      <c r="O54" s="34"/>
-      <c r="P54" s="39"/>
-      <c r="Q54" s="39"/>
+      <c r="E54" s="31"/>
+      <c r="F54" s="31"/>
+      <c r="G54" s="31"/>
+      <c r="H54" s="31"/>
+      <c r="I54" s="31"/>
+      <c r="J54" s="31"/>
+      <c r="K54" s="31"/>
+      <c r="L54" s="31"/>
+      <c r="M54" s="29"/>
+      <c r="N54" s="29"/>
+      <c r="O54" s="31"/>
+      <c r="P54" s="29"/>
+      <c r="Q54" s="29"/>
       <c r="R54" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="S54" s="39"/>
-      <c r="T54" s="39"/>
-      <c r="U54" s="39"/>
+      <c r="S54" s="29"/>
+      <c r="T54" s="29"/>
+      <c r="U54" s="29"/>
     </row>
     <row r="55" spans="1:21" ht="32" x14ac:dyDescent="0.2">
-      <c r="A55" s="36"/>
-      <c r="B55" s="32"/>
-      <c r="C55" s="32"/>
+      <c r="A55" s="34"/>
+      <c r="B55" s="35"/>
+      <c r="C55" s="35"/>
       <c r="D55" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="E55" s="34"/>
-      <c r="F55" s="34"/>
-      <c r="G55" s="34"/>
-      <c r="H55" s="34"/>
-      <c r="I55" s="34"/>
-      <c r="J55" s="34"/>
-      <c r="K55" s="34"/>
-      <c r="L55" s="34"/>
-      <c r="M55" s="39"/>
-      <c r="N55" s="39"/>
-      <c r="O55" s="34"/>
-      <c r="P55" s="39"/>
-      <c r="Q55" s="39"/>
+      <c r="E55" s="31"/>
+      <c r="F55" s="31"/>
+      <c r="G55" s="31"/>
+      <c r="H55" s="31"/>
+      <c r="I55" s="31"/>
+      <c r="J55" s="31"/>
+      <c r="K55" s="31"/>
+      <c r="L55" s="31"/>
+      <c r="M55" s="29"/>
+      <c r="N55" s="29"/>
+      <c r="O55" s="31"/>
+      <c r="P55" s="29"/>
+      <c r="Q55" s="29"/>
       <c r="R55" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="S55" s="39"/>
-      <c r="T55" s="39"/>
-      <c r="U55" s="39"/>
+      <c r="S55" s="29"/>
+      <c r="T55" s="29"/>
+      <c r="U55" s="29"/>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A56" s="24"/>
@@ -5108,78 +5111,20 @@
     </row>
   </sheetData>
   <mergeCells count="110">
-    <mergeCell ref="U10:U12"/>
-    <mergeCell ref="U26:U30"/>
-    <mergeCell ref="U31:U35"/>
-    <mergeCell ref="U36:U40"/>
-    <mergeCell ref="U41:U45"/>
-    <mergeCell ref="R46:R50"/>
-    <mergeCell ref="U46:U50"/>
-    <mergeCell ref="O46:O50"/>
-    <mergeCell ref="O51:O55"/>
-    <mergeCell ref="P51:P55"/>
-    <mergeCell ref="Q51:Q55"/>
-    <mergeCell ref="O26:O30"/>
-    <mergeCell ref="O31:O35"/>
-    <mergeCell ref="O36:O40"/>
-    <mergeCell ref="O41:O45"/>
-    <mergeCell ref="S51:S55"/>
-    <mergeCell ref="T51:T55"/>
-    <mergeCell ref="U51:U55"/>
-    <mergeCell ref="M26:M30"/>
-    <mergeCell ref="N26:N30"/>
-    <mergeCell ref="M36:M40"/>
-    <mergeCell ref="N36:N40"/>
-    <mergeCell ref="M46:M50"/>
-    <mergeCell ref="N46:N50"/>
-    <mergeCell ref="J51:J55"/>
-    <mergeCell ref="L36:L40"/>
-    <mergeCell ref="K51:K55"/>
-    <mergeCell ref="L51:L55"/>
-    <mergeCell ref="J36:J40"/>
-    <mergeCell ref="J41:J45"/>
-    <mergeCell ref="J46:J50"/>
-    <mergeCell ref="K31:K35"/>
-    <mergeCell ref="L31:L35"/>
-    <mergeCell ref="M51:M55"/>
-    <mergeCell ref="N51:N55"/>
-    <mergeCell ref="M31:M35"/>
-    <mergeCell ref="N31:N35"/>
-    <mergeCell ref="N41:N45"/>
-    <mergeCell ref="M41:M45"/>
-    <mergeCell ref="J10:J12"/>
-    <mergeCell ref="J13:J15"/>
-    <mergeCell ref="J26:J30"/>
-    <mergeCell ref="J31:J35"/>
-    <mergeCell ref="H10:H12"/>
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="H13:H15"/>
-    <mergeCell ref="I13:I15"/>
-    <mergeCell ref="H26:H30"/>
-    <mergeCell ref="I26:I30"/>
-    <mergeCell ref="H31:H35"/>
-    <mergeCell ref="G26:G30"/>
-    <mergeCell ref="G10:G12"/>
-    <mergeCell ref="G13:G15"/>
-    <mergeCell ref="E26:E30"/>
-    <mergeCell ref="F36:F40"/>
-    <mergeCell ref="F46:F50"/>
-    <mergeCell ref="E51:E55"/>
-    <mergeCell ref="F51:F55"/>
-    <mergeCell ref="G51:G55"/>
-    <mergeCell ref="G31:G35"/>
-    <mergeCell ref="G36:G40"/>
-    <mergeCell ref="G41:G45"/>
-    <mergeCell ref="G46:G50"/>
-    <mergeCell ref="E41:E45"/>
-    <mergeCell ref="F41:F45"/>
-    <mergeCell ref="E46:E50"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="E13:E15"/>
-    <mergeCell ref="F13:F15"/>
-    <mergeCell ref="F26:F30"/>
-    <mergeCell ref="E31:E35"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A6:D6"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
@@ -5204,20 +5149,78 @@
     <mergeCell ref="I51:I55"/>
     <mergeCell ref="F31:F35"/>
     <mergeCell ref="E36:E40"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="G26:G30"/>
+    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="G13:G15"/>
+    <mergeCell ref="E26:E30"/>
+    <mergeCell ref="F36:F40"/>
+    <mergeCell ref="F46:F50"/>
+    <mergeCell ref="E51:E55"/>
+    <mergeCell ref="F51:F55"/>
+    <mergeCell ref="G51:G55"/>
+    <mergeCell ref="G31:G35"/>
+    <mergeCell ref="G36:G40"/>
+    <mergeCell ref="G41:G45"/>
+    <mergeCell ref="G46:G50"/>
+    <mergeCell ref="E41:E45"/>
+    <mergeCell ref="F41:F45"/>
+    <mergeCell ref="E46:E50"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="F13:F15"/>
+    <mergeCell ref="F26:F30"/>
+    <mergeCell ref="E31:E35"/>
+    <mergeCell ref="J10:J12"/>
+    <mergeCell ref="J13:J15"/>
+    <mergeCell ref="J26:J30"/>
+    <mergeCell ref="J31:J35"/>
+    <mergeCell ref="H10:H12"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="H13:H15"/>
+    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="H26:H30"/>
+    <mergeCell ref="I26:I30"/>
+    <mergeCell ref="H31:H35"/>
+    <mergeCell ref="M26:M30"/>
+    <mergeCell ref="N26:N30"/>
+    <mergeCell ref="M36:M40"/>
+    <mergeCell ref="N36:N40"/>
+    <mergeCell ref="M46:M50"/>
+    <mergeCell ref="N46:N50"/>
+    <mergeCell ref="J51:J55"/>
+    <mergeCell ref="L36:L40"/>
+    <mergeCell ref="K51:K55"/>
+    <mergeCell ref="L51:L55"/>
+    <mergeCell ref="J36:J40"/>
+    <mergeCell ref="J41:J45"/>
+    <mergeCell ref="J46:J50"/>
+    <mergeCell ref="K31:K35"/>
+    <mergeCell ref="L31:L35"/>
+    <mergeCell ref="M51:M55"/>
+    <mergeCell ref="N51:N55"/>
+    <mergeCell ref="M31:M35"/>
+    <mergeCell ref="N31:N35"/>
+    <mergeCell ref="N41:N45"/>
+    <mergeCell ref="M41:M45"/>
+    <mergeCell ref="U10:U12"/>
+    <mergeCell ref="U26:U30"/>
+    <mergeCell ref="U31:U35"/>
+    <mergeCell ref="U36:U40"/>
+    <mergeCell ref="U41:U45"/>
+    <mergeCell ref="R46:R50"/>
+    <mergeCell ref="U46:U50"/>
+    <mergeCell ref="O46:O50"/>
+    <mergeCell ref="O51:O55"/>
+    <mergeCell ref="P51:P55"/>
+    <mergeCell ref="Q51:Q55"/>
+    <mergeCell ref="O26:O30"/>
+    <mergeCell ref="O31:O35"/>
+    <mergeCell ref="O36:O40"/>
+    <mergeCell ref="O41:O45"/>
+    <mergeCell ref="S51:S55"/>
+    <mergeCell ref="T51:T55"/>
+    <mergeCell ref="U51:U55"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="P2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Cleanup data from unused data and data for GRIP-GL
</commit_message>
<xml_diff>
--- a/data/Model_setups_GRIP.xlsx
+++ b/data/Model_setups_GRIP.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/j6mai/Documents/GitHub/GRIP-E/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/j6mai/Documents/GitHub/Publications/mai_GRIP-E/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41438857-5BF7-4C4C-9EB4-1E0D98D5B062}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E91198A-6E57-7744-87A1-3E9B8E82E555}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28800" yWindow="-700" windowWidth="28420" windowHeight="16280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="222">
   <si>
     <t>MODEL</t>
   </si>
@@ -710,9 +710,6 @@
   </si>
   <si>
     <t>USGS (GTOPO 30, 1996; for surface/soil slope computation); HydroSHEDS 1km (for delineation and routing); NHN/NHD (vector; for drainage density)</t>
-  </si>
-  <si>
-    <t>1- Global Soil Dataset for Earth System Models (GSDE); https://agupubs.onlinelibrary.wiley.com/doi/full/10.1002/2013MS000293, 2- Global Depth to Bedrock Dataset for Earth System Modeling (250m)performing aggregation using QGIS (zonal stats as done for GSDE) (http://globalchange.bnu.edu.cn/research/dtb.jsp)</t>
   </si>
 </sst>
 </file>
@@ -1026,8 +1023,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1038,14 +1044,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1053,11 +1053,8 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="109">
@@ -1509,10 +1506,10 @@
   <dimension ref="A1:U140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="N9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T11" sqref="T11"/>
+      <selection pane="bottomRight" activeCell="R132" sqref="R132:U140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1524,12 +1521,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
       <c r="E1" s="3" t="s">
         <v>199</v>
       </c>
@@ -1583,12 +1580,12 @@
       </c>
     </row>
     <row r="2" spans="1:21" ht="68" x14ac:dyDescent="0.2">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
       <c r="E2" s="25" t="s">
         <v>201</v>
       </c>
@@ -1642,12 +1639,12 @@
       </c>
     </row>
     <row r="3" spans="1:21" ht="51" x14ac:dyDescent="0.2">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
       <c r="E3" s="26" t="s">
         <v>189</v>
       </c>
@@ -1701,12 +1698,12 @@
       </c>
     </row>
     <row r="4" spans="1:21" ht="51" x14ac:dyDescent="0.2">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
       <c r="E4" s="25" t="s">
         <v>25</v>
       </c>
@@ -1760,12 +1757,12 @@
       </c>
     </row>
     <row r="5" spans="1:21" ht="85" x14ac:dyDescent="0.2">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
       <c r="E5" s="2" t="s">
         <v>207</v>
       </c>
@@ -1819,12 +1816,12 @@
       </c>
     </row>
     <row r="6" spans="1:21" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
       <c r="E6" s="25" t="s">
         <v>203</v>
       </c>
@@ -1878,14 +1875,14 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="102" x14ac:dyDescent="0.2">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
       <c r="E7" s="8" t="s">
         <v>53</v>
       </c>
@@ -1939,12 +1936,12 @@
       </c>
     </row>
     <row r="8" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="33"/>
-      <c r="B8" s="33" t="s">
+      <c r="A8" s="29"/>
+      <c r="B8" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
       <c r="E8" s="8" t="s">
         <v>54</v>
       </c>
@@ -1998,12 +1995,12 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="68" x14ac:dyDescent="0.2">
-      <c r="A9" s="33"/>
-      <c r="B9" s="33" t="s">
+      <c r="A9" s="29"/>
+      <c r="B9" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
       <c r="E9" s="26" t="s">
         <v>208</v>
       </c>
@@ -2049,30 +2046,30 @@
       <c r="U9" s="8"/>
     </row>
     <row r="10" spans="1:21" ht="255" x14ac:dyDescent="0.2">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="29" t="s">
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="39" t="s">
         <v>204</v>
       </c>
-      <c r="F10" s="29" t="s">
+      <c r="F10" s="39" t="s">
         <v>204</v>
       </c>
-      <c r="G10" s="29" t="s">
+      <c r="G10" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="29" t="s">
+      <c r="H10" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="I10" s="29" t="s">
+      <c r="I10" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="J10" s="29" t="s">
+      <c r="J10" s="39" t="s">
         <v>56</v>
       </c>
       <c r="K10" s="6" t="s">
@@ -2103,25 +2100,25 @@
         <v>170</v>
       </c>
       <c r="T10" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="U10" s="29" t="s">
+        <v>170</v>
+      </c>
+      <c r="U10" s="39" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="68" x14ac:dyDescent="0.2">
-      <c r="A11" s="38"/>
-      <c r="B11" s="38" t="s">
+      <c r="A11" s="30"/>
+      <c r="B11" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="29"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="39"/>
       <c r="K11" s="6" t="s">
         <v>80</v>
       </c>
@@ -2152,21 +2149,21 @@
       <c r="T11" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="U11" s="29"/>
+      <c r="U11" s="39"/>
     </row>
     <row r="12" spans="1:21" ht="119" x14ac:dyDescent="0.2">
-      <c r="A12" s="38"/>
-      <c r="B12" s="38" t="s">
+      <c r="A12" s="30"/>
+      <c r="B12" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="39"/>
       <c r="K12" s="10" t="s">
         <v>82</v>
       </c>
@@ -2197,33 +2194,33 @@
       <c r="T12" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="U12" s="29"/>
+      <c r="U12" s="39"/>
     </row>
     <row r="13" spans="1:21" ht="102" x14ac:dyDescent="0.2">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="32" t="s">
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="35" t="s">
         <v>205</v>
       </c>
-      <c r="F13" s="32" t="s">
+      <c r="F13" s="35" t="s">
         <v>205</v>
       </c>
-      <c r="G13" s="32" t="s">
+      <c r="G13" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="32" t="s">
+      <c r="H13" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="I13" s="32" t="s">
+      <c r="I13" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="J13" s="32" t="s">
+      <c r="J13" s="35" t="s">
         <v>67</v>
       </c>
       <c r="K13" s="2" t="s">
@@ -2261,18 +2258,18 @@
       </c>
     </row>
     <row r="14" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="33"/>
-      <c r="B14" s="33" t="s">
+      <c r="A14" s="29"/>
+      <c r="B14" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="32"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="35"/>
       <c r="K14" s="8" t="s">
         <v>84</v>
       </c>
@@ -2308,18 +2305,18 @@
       </c>
     </row>
     <row r="15" spans="1:21" ht="136" x14ac:dyDescent="0.2">
-      <c r="A15" s="33"/>
-      <c r="B15" s="33" t="s">
+      <c r="A15" s="29"/>
+      <c r="B15" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="35"/>
       <c r="K15" s="8"/>
       <c r="L15" s="8"/>
       <c r="M15" s="2" t="s">
@@ -2351,13 +2348,13 @@
       </c>
     </row>
     <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="35"/>
+      <c r="C16" s="32"/>
       <c r="D16" s="14" t="s">
         <v>14</v>
       </c>
@@ -2414,9 +2411,9 @@
       </c>
     </row>
     <row r="17" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="34"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="35"/>
+      <c r="A17" s="36"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
       <c r="D17" s="14" t="s">
         <v>46</v>
       </c>
@@ -2473,9 +2470,9 @@
       </c>
     </row>
     <row r="18" spans="1:21" ht="68" x14ac:dyDescent="0.2">
-      <c r="A18" s="34"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="35"/>
+      <c r="A18" s="36"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
       <c r="D18" s="14" t="s">
         <v>43</v>
       </c>
@@ -2528,9 +2525,9 @@
       </c>
     </row>
     <row r="19" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="34"/>
-      <c r="B19" s="35"/>
-      <c r="C19" s="35"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
       <c r="D19" s="14" t="s">
         <v>45</v>
       </c>
@@ -2587,9 +2584,9 @@
       </c>
     </row>
     <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="34"/>
-      <c r="B20" s="35"/>
-      <c r="C20" s="35"/>
+      <c r="A20" s="36"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
       <c r="D20" s="14" t="s">
         <v>44</v>
       </c>
@@ -2646,11 +2643,11 @@
       </c>
     </row>
     <row r="21" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="34"/>
-      <c r="B21" s="36" t="s">
+      <c r="A21" s="36"/>
+      <c r="B21" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="36"/>
+      <c r="C21" s="37"/>
       <c r="D21" s="16" t="s">
         <v>14</v>
       </c>
@@ -2707,9 +2704,9 @@
       </c>
     </row>
     <row r="22" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="34"/>
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
+      <c r="A22" s="36"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="37"/>
       <c r="D22" s="16" t="s">
         <v>46</v>
       </c>
@@ -2766,9 +2763,9 @@
       </c>
     </row>
     <row r="23" spans="1:21" ht="68" x14ac:dyDescent="0.2">
-      <c r="A23" s="34"/>
-      <c r="B23" s="36"/>
-      <c r="C23" s="36"/>
+      <c r="A23" s="36"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
       <c r="D23" s="16" t="s">
         <v>43</v>
       </c>
@@ -2821,9 +2818,9 @@
       </c>
     </row>
     <row r="24" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="34"/>
-      <c r="B24" s="36"/>
-      <c r="C24" s="36"/>
+      <c r="A24" s="36"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="37"/>
       <c r="D24" s="16" t="s">
         <v>45</v>
       </c>
@@ -2880,9 +2877,9 @@
       </c>
     </row>
     <row r="25" spans="1:21" ht="32" x14ac:dyDescent="0.2">
-      <c r="A25" s="34"/>
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
+      <c r="A25" s="36"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
       <c r="D25" s="16" t="s">
         <v>44</v>
       </c>
@@ -2939,30 +2936,30 @@
       </c>
     </row>
     <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="34"/>
-      <c r="B26" s="35" t="s">
+      <c r="A26" s="36"/>
+      <c r="B26" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="35"/>
+      <c r="C26" s="32"/>
       <c r="D26" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E26" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="F26" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="G26" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="H26" s="29" t="s">
+      <c r="E26" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="F26" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="G26" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="H26" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="I26" s="29" t="s">
+      <c r="I26" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="J26" s="31" t="s">
+      <c r="J26" s="34" t="s">
         <v>42</v>
       </c>
       <c r="K26" s="6" t="s">
@@ -2971,13 +2968,13 @@
       <c r="L26" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="M26" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="N26" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="O26" s="31" t="s">
+      <c r="M26" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="N26" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="O26" s="34" t="s">
         <v>42</v>
       </c>
       <c r="P26" s="6" t="s">
@@ -2995,32 +2992,32 @@
       <c r="T26" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="U26" s="29" t="s">
+      <c r="U26" s="39" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="34"/>
-      <c r="B27" s="35"/>
-      <c r="C27" s="35"/>
+      <c r="A27" s="36"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
       <c r="D27" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="29"/>
-      <c r="J27" s="31"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="39"/>
+      <c r="I27" s="39"/>
+      <c r="J27" s="34"/>
       <c r="K27" s="2" t="s">
         <v>34</v>
       </c>
       <c r="L27" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="M27" s="29"/>
-      <c r="N27" s="29"/>
-      <c r="O27" s="31"/>
+      <c r="M27" s="39"/>
+      <c r="N27" s="39"/>
+      <c r="O27" s="34"/>
       <c r="P27" s="10" t="s">
         <v>58</v>
       </c>
@@ -3036,30 +3033,30 @@
       <c r="T27" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="U27" s="29"/>
+      <c r="U27" s="39"/>
     </row>
     <row r="28" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="34"/>
-      <c r="B28" s="35"/>
-      <c r="C28" s="35"/>
+      <c r="A28" s="36"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
       <c r="D28" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="31"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="34"/>
       <c r="K28" s="5" t="s">
         <v>89</v>
       </c>
       <c r="L28" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="M28" s="29"/>
-      <c r="N28" s="29"/>
-      <c r="O28" s="31"/>
+      <c r="M28" s="39"/>
+      <c r="N28" s="39"/>
+      <c r="O28" s="34"/>
       <c r="P28" s="10" t="s">
         <v>59</v>
       </c>
@@ -3075,30 +3072,30 @@
       <c r="T28" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="U28" s="29"/>
+      <c r="U28" s="39"/>
     </row>
     <row r="29" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="34"/>
-      <c r="B29" s="35"/>
-      <c r="C29" s="35"/>
+      <c r="A29" s="36"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
       <c r="D29" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="29"/>
-      <c r="J29" s="31"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="34"/>
       <c r="K29" s="5" t="s">
         <v>90</v>
       </c>
       <c r="L29" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="M29" s="29"/>
-      <c r="N29" s="29"/>
-      <c r="O29" s="31"/>
+      <c r="M29" s="39"/>
+      <c r="N29" s="39"/>
+      <c r="O29" s="34"/>
       <c r="P29" s="6" t="s">
         <v>147</v>
       </c>
@@ -3114,30 +3111,30 @@
       <c r="T29" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="U29" s="29"/>
+      <c r="U29" s="39"/>
     </row>
     <row r="30" spans="1:21" ht="32" x14ac:dyDescent="0.2">
-      <c r="A30" s="34"/>
-      <c r="B30" s="35"/>
-      <c r="C30" s="35"/>
+      <c r="A30" s="36"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
       <c r="D30" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="29"/>
-      <c r="J30" s="31"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="34"/>
       <c r="K30" s="5" t="s">
         <v>91</v>
       </c>
       <c r="L30" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="M30" s="29"/>
-      <c r="N30" s="29"/>
-      <c r="O30" s="31"/>
+      <c r="M30" s="39"/>
+      <c r="N30" s="39"/>
+      <c r="O30" s="34"/>
       <c r="P30" s="5" t="s">
         <v>37</v>
       </c>
@@ -3153,48 +3150,48 @@
       <c r="T30" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="U30" s="29"/>
+      <c r="U30" s="39"/>
     </row>
     <row r="31" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="34"/>
-      <c r="B31" s="36" t="s">
+      <c r="A31" s="36"/>
+      <c r="B31" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="36"/>
+      <c r="C31" s="37"/>
       <c r="D31" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E31" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="F31" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="G31" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="H31" s="30" t="s">
+      <c r="E31" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="F31" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="G31" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="H31" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="I31" s="30" t="s">
+      <c r="I31" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="J31" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="K31" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="L31" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="M31" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="N31" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="O31" s="30" t="s">
+      <c r="J31" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="K31" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="L31" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="M31" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="N31" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="O31" s="33" t="s">
         <v>42</v>
       </c>
       <c r="P31" s="8" t="s">
@@ -3212,28 +3209,28 @@
       <c r="T31" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="U31" s="30" t="s">
+      <c r="U31" s="33" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="34"/>
-      <c r="B32" s="36"/>
-      <c r="C32" s="36"/>
+      <c r="A32" s="36"/>
+      <c r="B32" s="37"/>
+      <c r="C32" s="37"/>
       <c r="D32" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="E32" s="30"/>
-      <c r="F32" s="30"/>
-      <c r="G32" s="30"/>
-      <c r="H32" s="30"/>
-      <c r="I32" s="30"/>
-      <c r="J32" s="32"/>
-      <c r="K32" s="32"/>
-      <c r="L32" s="32"/>
-      <c r="M32" s="32"/>
-      <c r="N32" s="32"/>
-      <c r="O32" s="30"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="33"/>
+      <c r="I32" s="33"/>
+      <c r="J32" s="35"/>
+      <c r="K32" s="35"/>
+      <c r="L32" s="35"/>
+      <c r="M32" s="35"/>
+      <c r="N32" s="35"/>
+      <c r="O32" s="33"/>
       <c r="P32" s="8" t="s">
         <v>87</v>
       </c>
@@ -3249,26 +3246,26 @@
       <c r="T32" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="U32" s="30"/>
+      <c r="U32" s="33"/>
     </row>
     <row r="33" spans="1:21" ht="32" x14ac:dyDescent="0.2">
-      <c r="A33" s="34"/>
-      <c r="B33" s="36"/>
-      <c r="C33" s="36"/>
+      <c r="A33" s="36"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="37"/>
       <c r="D33" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="E33" s="30"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="30"/>
-      <c r="I33" s="30"/>
-      <c r="J33" s="32"/>
-      <c r="K33" s="32"/>
-      <c r="L33" s="32"/>
-      <c r="M33" s="32"/>
-      <c r="N33" s="32"/>
-      <c r="O33" s="30"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="33"/>
+      <c r="H33" s="33"/>
+      <c r="I33" s="33"/>
+      <c r="J33" s="35"/>
+      <c r="K33" s="35"/>
+      <c r="L33" s="35"/>
+      <c r="M33" s="35"/>
+      <c r="N33" s="35"/>
+      <c r="O33" s="33"/>
       <c r="P33" s="8" t="s">
         <v>59</v>
       </c>
@@ -3284,26 +3281,26 @@
       <c r="T33" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="U33" s="30"/>
+      <c r="U33" s="33"/>
     </row>
     <row r="34" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="34"/>
-      <c r="B34" s="36"/>
-      <c r="C34" s="36"/>
+      <c r="A34" s="36"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="37"/>
       <c r="D34" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="E34" s="30"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="30"/>
-      <c r="I34" s="30"/>
-      <c r="J34" s="32"/>
-      <c r="K34" s="32"/>
-      <c r="L34" s="32"/>
-      <c r="M34" s="32"/>
-      <c r="N34" s="32"/>
-      <c r="O34" s="30"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="33"/>
+      <c r="H34" s="33"/>
+      <c r="I34" s="33"/>
+      <c r="J34" s="35"/>
+      <c r="K34" s="35"/>
+      <c r="L34" s="35"/>
+      <c r="M34" s="35"/>
+      <c r="N34" s="35"/>
+      <c r="O34" s="33"/>
       <c r="P34" s="8" t="s">
         <v>147</v>
       </c>
@@ -3319,26 +3316,26 @@
       <c r="T34" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="U34" s="30"/>
+      <c r="U34" s="33"/>
     </row>
     <row r="35" spans="1:21" ht="32" x14ac:dyDescent="0.2">
-      <c r="A35" s="34"/>
-      <c r="B35" s="36"/>
-      <c r="C35" s="36"/>
+      <c r="A35" s="36"/>
+      <c r="B35" s="37"/>
+      <c r="C35" s="37"/>
       <c r="D35" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="E35" s="30"/>
-      <c r="F35" s="30"/>
-      <c r="G35" s="30"/>
-      <c r="H35" s="30"/>
-      <c r="I35" s="30"/>
-      <c r="J35" s="32"/>
-      <c r="K35" s="32"/>
-      <c r="L35" s="32"/>
-      <c r="M35" s="32"/>
-      <c r="N35" s="32"/>
-      <c r="O35" s="30"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="33"/>
+      <c r="H35" s="33"/>
+      <c r="I35" s="33"/>
+      <c r="J35" s="35"/>
+      <c r="K35" s="35"/>
+      <c r="L35" s="35"/>
+      <c r="M35" s="35"/>
+      <c r="N35" s="35"/>
+      <c r="O35" s="33"/>
       <c r="P35" s="8" t="s">
         <v>37</v>
       </c>
@@ -3354,48 +3351,48 @@
       <c r="T35" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="U35" s="30"/>
+      <c r="U35" s="33"/>
     </row>
     <row r="36" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="34"/>
-      <c r="B36" s="35" t="s">
+      <c r="A36" s="36"/>
+      <c r="B36" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="35"/>
+      <c r="C36" s="32"/>
       <c r="D36" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E36" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="F36" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="G36" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="H36" s="31" t="s">
+      <c r="E36" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="F36" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="G36" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="H36" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="I36" s="31" t="s">
+      <c r="I36" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="J36" s="31" t="s">
+      <c r="J36" s="34" t="s">
         <v>42</v>
       </c>
       <c r="K36" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="L36" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="M36" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="N36" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="O36" s="31" t="s">
+      <c r="L36" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="M36" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="N36" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="O36" s="34" t="s">
         <v>42</v>
       </c>
       <c r="P36" s="6" t="s">
@@ -3413,30 +3410,30 @@
       <c r="T36" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="U36" s="29" t="s">
+      <c r="U36" s="39" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="34"/>
-      <c r="B37" s="35"/>
-      <c r="C37" s="35"/>
+      <c r="A37" s="36"/>
+      <c r="B37" s="32"/>
+      <c r="C37" s="32"/>
       <c r="D37" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
-      <c r="G37" s="31"/>
-      <c r="H37" s="31"/>
-      <c r="I37" s="31"/>
-      <c r="J37" s="31"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
+      <c r="G37" s="34"/>
+      <c r="H37" s="34"/>
+      <c r="I37" s="34"/>
+      <c r="J37" s="34"/>
       <c r="K37" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="L37" s="31"/>
-      <c r="M37" s="29"/>
-      <c r="N37" s="29"/>
-      <c r="O37" s="31"/>
+      <c r="L37" s="34"/>
+      <c r="M37" s="39"/>
+      <c r="N37" s="39"/>
+      <c r="O37" s="34"/>
       <c r="P37" s="10" t="s">
         <v>87</v>
       </c>
@@ -3452,26 +3449,26 @@
       <c r="T37" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="U37" s="29"/>
+      <c r="U37" s="39"/>
     </row>
     <row r="38" spans="1:21" ht="34" x14ac:dyDescent="0.2">
-      <c r="A38" s="34"/>
-      <c r="B38" s="35"/>
-      <c r="C38" s="35"/>
+      <c r="A38" s="36"/>
+      <c r="B38" s="32"/>
+      <c r="C38" s="32"/>
       <c r="D38" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="E38" s="31"/>
-      <c r="F38" s="31"/>
-      <c r="G38" s="31"/>
-      <c r="H38" s="31"/>
-      <c r="I38" s="31"/>
-      <c r="J38" s="31"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="34"/>
+      <c r="G38" s="34"/>
+      <c r="H38" s="34"/>
+      <c r="I38" s="34"/>
+      <c r="J38" s="34"/>
       <c r="K38" s="5"/>
-      <c r="L38" s="31"/>
-      <c r="M38" s="29"/>
-      <c r="N38" s="29"/>
-      <c r="O38" s="31"/>
+      <c r="L38" s="34"/>
+      <c r="M38" s="39"/>
+      <c r="N38" s="39"/>
+      <c r="O38" s="34"/>
       <c r="P38" s="10" t="s">
         <v>59</v>
       </c>
@@ -3487,28 +3484,28 @@
       <c r="T38" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="U38" s="29"/>
+      <c r="U38" s="39"/>
     </row>
     <row r="39" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="34"/>
-      <c r="B39" s="35"/>
-      <c r="C39" s="35"/>
+      <c r="A39" s="36"/>
+      <c r="B39" s="32"/>
+      <c r="C39" s="32"/>
       <c r="D39" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E39" s="31"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="31"/>
-      <c r="H39" s="31"/>
-      <c r="I39" s="31"/>
-      <c r="J39" s="31"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="34"/>
+      <c r="G39" s="34"/>
+      <c r="H39" s="34"/>
+      <c r="I39" s="34"/>
+      <c r="J39" s="34"/>
       <c r="K39" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="L39" s="31"/>
-      <c r="M39" s="29"/>
-      <c r="N39" s="29"/>
-      <c r="O39" s="31"/>
+      <c r="L39" s="34"/>
+      <c r="M39" s="39"/>
+      <c r="N39" s="39"/>
+      <c r="O39" s="34"/>
       <c r="P39" s="5" t="s">
         <v>148</v>
       </c>
@@ -3524,28 +3521,28 @@
       <c r="T39" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="U39" s="29"/>
+      <c r="U39" s="39"/>
     </row>
     <row r="40" spans="1:21" ht="32" x14ac:dyDescent="0.2">
-      <c r="A40" s="34"/>
-      <c r="B40" s="35"/>
-      <c r="C40" s="35"/>
+      <c r="A40" s="36"/>
+      <c r="B40" s="32"/>
+      <c r="C40" s="32"/>
       <c r="D40" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="E40" s="31"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="31"/>
-      <c r="H40" s="31"/>
-      <c r="I40" s="31"/>
-      <c r="J40" s="31"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="34"/>
+      <c r="G40" s="34"/>
+      <c r="H40" s="34"/>
+      <c r="I40" s="34"/>
+      <c r="J40" s="34"/>
       <c r="K40" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="L40" s="31"/>
-      <c r="M40" s="29"/>
-      <c r="N40" s="29"/>
-      <c r="O40" s="31"/>
+      <c r="L40" s="34"/>
+      <c r="M40" s="39"/>
+      <c r="N40" s="39"/>
+      <c r="O40" s="34"/>
       <c r="P40" s="5" t="s">
         <v>149</v>
       </c>
@@ -3561,33 +3558,33 @@
       <c r="T40" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="U40" s="29"/>
+      <c r="U40" s="39"/>
     </row>
     <row r="41" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="34"/>
-      <c r="B41" s="36" t="s">
+      <c r="A41" s="36"/>
+      <c r="B41" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="C41" s="36"/>
+      <c r="C41" s="37"/>
       <c r="D41" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E41" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="F41" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="G41" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="H41" s="32" t="s">
+      <c r="E41" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="F41" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="G41" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="H41" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="I41" s="32" t="s">
+      <c r="I41" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="J41" s="30" t="s">
+      <c r="J41" s="33" t="s">
         <v>42</v>
       </c>
       <c r="K41" s="2" t="s">
@@ -3596,13 +3593,13 @@
       <c r="L41" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="M41" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="N41" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="O41" s="30" t="s">
+      <c r="M41" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="N41" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="O41" s="33" t="s">
         <v>42</v>
       </c>
       <c r="P41" s="8" t="s">
@@ -3620,32 +3617,32 @@
       <c r="T41" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="U41" s="30" t="s">
+      <c r="U41" s="33" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="42" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="34"/>
-      <c r="B42" s="36"/>
-      <c r="C42" s="36"/>
+      <c r="A42" s="36"/>
+      <c r="B42" s="37"/>
+      <c r="C42" s="37"/>
       <c r="D42" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="E42" s="30"/>
-      <c r="F42" s="30"/>
-      <c r="G42" s="30"/>
-      <c r="H42" s="32"/>
-      <c r="I42" s="32"/>
-      <c r="J42" s="30"/>
+      <c r="E42" s="33"/>
+      <c r="F42" s="33"/>
+      <c r="G42" s="33"/>
+      <c r="H42" s="35"/>
+      <c r="I42" s="35"/>
+      <c r="J42" s="33"/>
       <c r="K42" s="2" t="s">
         <v>34</v>
       </c>
       <c r="L42" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="M42" s="32"/>
-      <c r="N42" s="32"/>
-      <c r="O42" s="30"/>
+      <c r="M42" s="35"/>
+      <c r="N42" s="35"/>
+      <c r="O42" s="33"/>
       <c r="P42" s="8" t="s">
         <v>87</v>
       </c>
@@ -3661,30 +3658,30 @@
       <c r="T42" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="U42" s="30"/>
+      <c r="U42" s="33"/>
     </row>
     <row r="43" spans="1:21" ht="48" x14ac:dyDescent="0.2">
-      <c r="A43" s="34"/>
-      <c r="B43" s="36"/>
-      <c r="C43" s="36"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="37"/>
+      <c r="C43" s="37"/>
       <c r="D43" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="E43" s="30"/>
-      <c r="F43" s="30"/>
-      <c r="G43" s="30"/>
-      <c r="H43" s="32"/>
-      <c r="I43" s="32"/>
-      <c r="J43" s="30"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="33"/>
+      <c r="G43" s="33"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="33"/>
       <c r="K43" s="18" t="s">
         <v>94</v>
       </c>
       <c r="L43" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="M43" s="32"/>
-      <c r="N43" s="32"/>
-      <c r="O43" s="30"/>
+      <c r="M43" s="35"/>
+      <c r="N43" s="35"/>
+      <c r="O43" s="33"/>
       <c r="P43" s="8" t="s">
         <v>150</v>
       </c>
@@ -3700,30 +3697,30 @@
       <c r="T43" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="U43" s="30"/>
+      <c r="U43" s="33"/>
     </row>
     <row r="44" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="34"/>
-      <c r="B44" s="36"/>
-      <c r="C44" s="36"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="37"/>
+      <c r="C44" s="37"/>
       <c r="D44" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="E44" s="30"/>
-      <c r="F44" s="30"/>
-      <c r="G44" s="30"/>
-      <c r="H44" s="32"/>
-      <c r="I44" s="32"/>
-      <c r="J44" s="30"/>
+      <c r="E44" s="33"/>
+      <c r="F44" s="33"/>
+      <c r="G44" s="33"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="33"/>
       <c r="K44" s="2" t="s">
         <v>95</v>
       </c>
       <c r="L44" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="M44" s="32"/>
-      <c r="N44" s="32"/>
-      <c r="O44" s="30"/>
+      <c r="M44" s="35"/>
+      <c r="N44" s="35"/>
+      <c r="O44" s="33"/>
       <c r="P44" s="8" t="s">
         <v>148</v>
       </c>
@@ -3739,30 +3736,30 @@
       <c r="T44" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="U44" s="30"/>
+      <c r="U44" s="33"/>
     </row>
     <row r="45" spans="1:21" ht="68" x14ac:dyDescent="0.2">
-      <c r="A45" s="34"/>
-      <c r="B45" s="36"/>
-      <c r="C45" s="36"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="37"/>
+      <c r="C45" s="37"/>
       <c r="D45" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="E45" s="30"/>
-      <c r="F45" s="30"/>
-      <c r="G45" s="30"/>
-      <c r="H45" s="32"/>
-      <c r="I45" s="32"/>
-      <c r="J45" s="30"/>
+      <c r="E45" s="33"/>
+      <c r="F45" s="33"/>
+      <c r="G45" s="33"/>
+      <c r="H45" s="35"/>
+      <c r="I45" s="35"/>
+      <c r="J45" s="33"/>
       <c r="K45" s="2" t="s">
         <v>96</v>
       </c>
       <c r="L45" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="M45" s="32"/>
-      <c r="N45" s="32"/>
-      <c r="O45" s="30"/>
+      <c r="M45" s="35"/>
+      <c r="N45" s="35"/>
+      <c r="O45" s="33"/>
       <c r="P45" s="8" t="s">
         <v>151</v>
       </c>
@@ -3778,33 +3775,33 @@
       <c r="T45" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="U45" s="30"/>
+      <c r="U45" s="33"/>
     </row>
     <row r="46" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" s="34"/>
-      <c r="B46" s="35" t="s">
+      <c r="A46" s="36"/>
+      <c r="B46" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C46" s="35"/>
+      <c r="C46" s="32"/>
       <c r="D46" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E46" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="F46" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="G46" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="H46" s="37" t="s">
+      <c r="E46" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="F46" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="G46" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="H46" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="I46" s="37" t="s">
+      <c r="I46" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="J46" s="31" t="s">
+      <c r="J46" s="34" t="s">
         <v>42</v>
       </c>
       <c r="K46" s="11" t="s">
@@ -3813,13 +3810,13 @@
       <c r="L46" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="M46" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="N46" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="O46" s="31" t="s">
+      <c r="M46" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="N46" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="O46" s="34" t="s">
         <v>42</v>
       </c>
       <c r="P46" s="10" t="s">
@@ -3828,7 +3825,7 @@
       <c r="Q46" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="R46" s="29" t="s">
+      <c r="R46" s="39" t="s">
         <v>42</v>
       </c>
       <c r="S46" s="6" t="s">
@@ -3837,326 +3834,326 @@
       <c r="T46" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="U46" s="29" t="s">
+      <c r="U46" s="39" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" s="34"/>
-      <c r="B47" s="35"/>
-      <c r="C47" s="35"/>
+      <c r="A47" s="36"/>
+      <c r="B47" s="32"/>
+      <c r="C47" s="32"/>
       <c r="D47" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="E47" s="31"/>
-      <c r="F47" s="31"/>
-      <c r="G47" s="31"/>
-      <c r="H47" s="37"/>
-      <c r="I47" s="37"/>
-      <c r="J47" s="31"/>
+      <c r="E47" s="34"/>
+      <c r="F47" s="34"/>
+      <c r="G47" s="34"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="38"/>
+      <c r="J47" s="34"/>
       <c r="K47" s="11" t="s">
         <v>34</v>
       </c>
       <c r="L47" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="M47" s="29"/>
-      <c r="N47" s="29"/>
-      <c r="O47" s="31"/>
+      <c r="M47" s="39"/>
+      <c r="N47" s="39"/>
+      <c r="O47" s="34"/>
       <c r="P47" s="10" t="s">
         <v>58</v>
       </c>
       <c r="Q47" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="R47" s="29"/>
+      <c r="R47" s="39"/>
       <c r="S47" s="6" t="s">
         <v>174</v>
       </c>
       <c r="T47" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="U47" s="29"/>
+      <c r="U47" s="39"/>
     </row>
     <row r="48" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="34"/>
-      <c r="B48" s="35"/>
-      <c r="C48" s="35"/>
+      <c r="A48" s="36"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="32"/>
       <c r="D48" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="E48" s="31"/>
-      <c r="F48" s="31"/>
-      <c r="G48" s="31"/>
-      <c r="H48" s="37"/>
-      <c r="I48" s="37"/>
-      <c r="J48" s="31"/>
+      <c r="E48" s="34"/>
+      <c r="F48" s="34"/>
+      <c r="G48" s="34"/>
+      <c r="H48" s="38"/>
+      <c r="I48" s="38"/>
+      <c r="J48" s="34"/>
       <c r="K48" s="11" t="s">
         <v>98</v>
       </c>
       <c r="L48" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="M48" s="29"/>
-      <c r="N48" s="29"/>
-      <c r="O48" s="31"/>
+      <c r="M48" s="39"/>
+      <c r="N48" s="39"/>
+      <c r="O48" s="34"/>
       <c r="P48" s="10" t="s">
         <v>152</v>
       </c>
       <c r="Q48" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="R48" s="29"/>
+      <c r="R48" s="39"/>
       <c r="S48" s="6" t="s">
         <v>196</v>
       </c>
       <c r="T48" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="U48" s="29"/>
+      <c r="U48" s="39"/>
     </row>
     <row r="49" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="A49" s="34"/>
-      <c r="B49" s="35"/>
-      <c r="C49" s="35"/>
+      <c r="A49" s="36"/>
+      <c r="B49" s="32"/>
+      <c r="C49" s="32"/>
       <c r="D49" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E49" s="31"/>
-      <c r="F49" s="31"/>
-      <c r="G49" s="31"/>
-      <c r="H49" s="37"/>
-      <c r="I49" s="37"/>
-      <c r="J49" s="31"/>
+      <c r="E49" s="34"/>
+      <c r="F49" s="34"/>
+      <c r="G49" s="34"/>
+      <c r="H49" s="38"/>
+      <c r="I49" s="38"/>
+      <c r="J49" s="34"/>
       <c r="K49" s="11" t="s">
         <v>99</v>
       </c>
       <c r="L49" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="M49" s="29"/>
-      <c r="N49" s="29"/>
-      <c r="O49" s="31"/>
+      <c r="M49" s="39"/>
+      <c r="N49" s="39"/>
+      <c r="O49" s="34"/>
       <c r="P49" s="6" t="s">
         <v>153</v>
       </c>
       <c r="Q49" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="R49" s="29"/>
+      <c r="R49" s="39"/>
       <c r="S49" s="6" t="s">
         <v>153</v>
       </c>
       <c r="T49" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="U49" s="29"/>
+      <c r="U49" s="39"/>
     </row>
     <row r="50" spans="1:21" ht="32" x14ac:dyDescent="0.2">
-      <c r="A50" s="34"/>
-      <c r="B50" s="35"/>
-      <c r="C50" s="35"/>
+      <c r="A50" s="36"/>
+      <c r="B50" s="32"/>
+      <c r="C50" s="32"/>
       <c r="D50" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="E50" s="31"/>
-      <c r="F50" s="31"/>
-      <c r="G50" s="31"/>
-      <c r="H50" s="37"/>
-      <c r="I50" s="37"/>
-      <c r="J50" s="31"/>
+      <c r="E50" s="34"/>
+      <c r="F50" s="34"/>
+      <c r="G50" s="34"/>
+      <c r="H50" s="38"/>
+      <c r="I50" s="38"/>
+      <c r="J50" s="34"/>
       <c r="K50" s="11" t="s">
         <v>100</v>
       </c>
       <c r="L50" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="M50" s="29"/>
-      <c r="N50" s="29"/>
-      <c r="O50" s="31"/>
+      <c r="M50" s="39"/>
+      <c r="N50" s="39"/>
+      <c r="O50" s="34"/>
       <c r="P50" s="6" t="s">
         <v>154</v>
       </c>
       <c r="Q50" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="R50" s="29"/>
+      <c r="R50" s="39"/>
       <c r="S50" s="6" t="s">
         <v>154</v>
       </c>
       <c r="T50" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="U50" s="29"/>
+      <c r="U50" s="39"/>
     </row>
     <row r="51" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="34"/>
-      <c r="B51" s="35" t="s">
+      <c r="A51" s="36"/>
+      <c r="B51" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="C51" s="35"/>
+      <c r="C51" s="32"/>
       <c r="D51" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E51" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="F51" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="G51" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="H51" s="31" t="s">
+      <c r="E51" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="F51" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="G51" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="H51" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="I51" s="31" t="s">
+      <c r="I51" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="J51" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="K51" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="L51" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="M51" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="N51" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="O51" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="P51" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q51" s="29" t="s">
+      <c r="J51" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="K51" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="L51" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="M51" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="N51" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="O51" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="P51" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q51" s="39" t="s">
         <v>42</v>
       </c>
       <c r="R51" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="S51" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="T51" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="U51" s="29" t="s">
+      <c r="S51" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="T51" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="U51" s="39" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="52" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="A52" s="34"/>
-      <c r="B52" s="35"/>
-      <c r="C52" s="35"/>
+      <c r="A52" s="36"/>
+      <c r="B52" s="32"/>
+      <c r="C52" s="32"/>
       <c r="D52" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="E52" s="31"/>
-      <c r="F52" s="31"/>
-      <c r="G52" s="31"/>
-      <c r="H52" s="31"/>
-      <c r="I52" s="31"/>
-      <c r="J52" s="31"/>
-      <c r="K52" s="31"/>
-      <c r="L52" s="31"/>
-      <c r="M52" s="29"/>
-      <c r="N52" s="29"/>
-      <c r="O52" s="31"/>
-      <c r="P52" s="29"/>
-      <c r="Q52" s="29"/>
+      <c r="E52" s="34"/>
+      <c r="F52" s="34"/>
+      <c r="G52" s="34"/>
+      <c r="H52" s="34"/>
+      <c r="I52" s="34"/>
+      <c r="J52" s="34"/>
+      <c r="K52" s="34"/>
+      <c r="L52" s="34"/>
+      <c r="M52" s="39"/>
+      <c r="N52" s="39"/>
+      <c r="O52" s="34"/>
+      <c r="P52" s="39"/>
+      <c r="Q52" s="39"/>
       <c r="R52" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="S52" s="29"/>
-      <c r="T52" s="29"/>
-      <c r="U52" s="29"/>
+      <c r="S52" s="39"/>
+      <c r="T52" s="39"/>
+      <c r="U52" s="39"/>
     </row>
     <row r="53" spans="1:21" ht="34" x14ac:dyDescent="0.2">
-      <c r="A53" s="34"/>
-      <c r="B53" s="35"/>
-      <c r="C53" s="35"/>
+      <c r="A53" s="36"/>
+      <c r="B53" s="32"/>
+      <c r="C53" s="32"/>
       <c r="D53" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="E53" s="31"/>
-      <c r="F53" s="31"/>
-      <c r="G53" s="31"/>
-      <c r="H53" s="31"/>
-      <c r="I53" s="31"/>
-      <c r="J53" s="31"/>
-      <c r="K53" s="31"/>
-      <c r="L53" s="31"/>
-      <c r="M53" s="29"/>
-      <c r="N53" s="29"/>
-      <c r="O53" s="31"/>
-      <c r="P53" s="29"/>
-      <c r="Q53" s="29"/>
+      <c r="E53" s="34"/>
+      <c r="F53" s="34"/>
+      <c r="G53" s="34"/>
+      <c r="H53" s="34"/>
+      <c r="I53" s="34"/>
+      <c r="J53" s="34"/>
+      <c r="K53" s="34"/>
+      <c r="L53" s="34"/>
+      <c r="M53" s="39"/>
+      <c r="N53" s="39"/>
+      <c r="O53" s="34"/>
+      <c r="P53" s="39"/>
+      <c r="Q53" s="39"/>
       <c r="R53" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="S53" s="29"/>
-      <c r="T53" s="29"/>
-      <c r="U53" s="29"/>
+      <c r="S53" s="39"/>
+      <c r="T53" s="39"/>
+      <c r="U53" s="39"/>
     </row>
     <row r="54" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="A54" s="34"/>
-      <c r="B54" s="35"/>
-      <c r="C54" s="35"/>
+      <c r="A54" s="36"/>
+      <c r="B54" s="32"/>
+      <c r="C54" s="32"/>
       <c r="D54" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E54" s="31"/>
-      <c r="F54" s="31"/>
-      <c r="G54" s="31"/>
-      <c r="H54" s="31"/>
-      <c r="I54" s="31"/>
-      <c r="J54" s="31"/>
-      <c r="K54" s="31"/>
-      <c r="L54" s="31"/>
-      <c r="M54" s="29"/>
-      <c r="N54" s="29"/>
-      <c r="O54" s="31"/>
-      <c r="P54" s="29"/>
-      <c r="Q54" s="29"/>
+      <c r="E54" s="34"/>
+      <c r="F54" s="34"/>
+      <c r="G54" s="34"/>
+      <c r="H54" s="34"/>
+      <c r="I54" s="34"/>
+      <c r="J54" s="34"/>
+      <c r="K54" s="34"/>
+      <c r="L54" s="34"/>
+      <c r="M54" s="39"/>
+      <c r="N54" s="39"/>
+      <c r="O54" s="34"/>
+      <c r="P54" s="39"/>
+      <c r="Q54" s="39"/>
       <c r="R54" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="S54" s="29"/>
-      <c r="T54" s="29"/>
-      <c r="U54" s="29"/>
+      <c r="S54" s="39"/>
+      <c r="T54" s="39"/>
+      <c r="U54" s="39"/>
     </row>
     <row r="55" spans="1:21" ht="32" x14ac:dyDescent="0.2">
-      <c r="A55" s="34"/>
-      <c r="B55" s="35"/>
-      <c r="C55" s="35"/>
+      <c r="A55" s="36"/>
+      <c r="B55" s="32"/>
+      <c r="C55" s="32"/>
       <c r="D55" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="E55" s="31"/>
-      <c r="F55" s="31"/>
-      <c r="G55" s="31"/>
-      <c r="H55" s="31"/>
-      <c r="I55" s="31"/>
-      <c r="J55" s="31"/>
-      <c r="K55" s="31"/>
-      <c r="L55" s="31"/>
-      <c r="M55" s="29"/>
-      <c r="N55" s="29"/>
-      <c r="O55" s="31"/>
-      <c r="P55" s="29"/>
-      <c r="Q55" s="29"/>
+      <c r="E55" s="34"/>
+      <c r="F55" s="34"/>
+      <c r="G55" s="34"/>
+      <c r="H55" s="34"/>
+      <c r="I55" s="34"/>
+      <c r="J55" s="34"/>
+      <c r="K55" s="34"/>
+      <c r="L55" s="34"/>
+      <c r="M55" s="39"/>
+      <c r="N55" s="39"/>
+      <c r="O55" s="34"/>
+      <c r="P55" s="39"/>
+      <c r="Q55" s="39"/>
       <c r="R55" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="S55" s="29"/>
-      <c r="T55" s="29"/>
-      <c r="U55" s="29"/>
+      <c r="S55" s="39"/>
+      <c r="T55" s="39"/>
+      <c r="U55" s="39"/>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A56" s="24"/>
@@ -5111,20 +5108,78 @@
     </row>
   </sheetData>
   <mergeCells count="110">
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="U10:U12"/>
+    <mergeCell ref="U26:U30"/>
+    <mergeCell ref="U31:U35"/>
+    <mergeCell ref="U36:U40"/>
+    <mergeCell ref="U41:U45"/>
+    <mergeCell ref="R46:R50"/>
+    <mergeCell ref="U46:U50"/>
+    <mergeCell ref="O46:O50"/>
+    <mergeCell ref="O51:O55"/>
+    <mergeCell ref="P51:P55"/>
+    <mergeCell ref="Q51:Q55"/>
+    <mergeCell ref="O26:O30"/>
+    <mergeCell ref="O31:O35"/>
+    <mergeCell ref="O36:O40"/>
+    <mergeCell ref="O41:O45"/>
+    <mergeCell ref="S51:S55"/>
+    <mergeCell ref="T51:T55"/>
+    <mergeCell ref="U51:U55"/>
+    <mergeCell ref="M26:M30"/>
+    <mergeCell ref="N26:N30"/>
+    <mergeCell ref="M36:M40"/>
+    <mergeCell ref="N36:N40"/>
+    <mergeCell ref="M46:M50"/>
+    <mergeCell ref="N46:N50"/>
+    <mergeCell ref="J51:J55"/>
+    <mergeCell ref="L36:L40"/>
+    <mergeCell ref="K51:K55"/>
+    <mergeCell ref="L51:L55"/>
+    <mergeCell ref="J36:J40"/>
+    <mergeCell ref="J41:J45"/>
+    <mergeCell ref="J46:J50"/>
+    <mergeCell ref="K31:K35"/>
+    <mergeCell ref="L31:L35"/>
+    <mergeCell ref="M51:M55"/>
+    <mergeCell ref="N51:N55"/>
+    <mergeCell ref="M31:M35"/>
+    <mergeCell ref="N31:N35"/>
+    <mergeCell ref="N41:N45"/>
+    <mergeCell ref="M41:M45"/>
+    <mergeCell ref="J10:J12"/>
+    <mergeCell ref="J13:J15"/>
+    <mergeCell ref="J26:J30"/>
+    <mergeCell ref="J31:J35"/>
+    <mergeCell ref="H10:H12"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="H13:H15"/>
+    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="H26:H30"/>
+    <mergeCell ref="I26:I30"/>
+    <mergeCell ref="H31:H35"/>
+    <mergeCell ref="G26:G30"/>
+    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="G13:G15"/>
+    <mergeCell ref="E26:E30"/>
+    <mergeCell ref="F36:F40"/>
+    <mergeCell ref="F46:F50"/>
+    <mergeCell ref="E51:E55"/>
+    <mergeCell ref="F51:F55"/>
+    <mergeCell ref="G51:G55"/>
+    <mergeCell ref="G31:G35"/>
+    <mergeCell ref="G36:G40"/>
+    <mergeCell ref="G41:G45"/>
+    <mergeCell ref="G46:G50"/>
+    <mergeCell ref="E41:E45"/>
+    <mergeCell ref="F41:F45"/>
+    <mergeCell ref="E46:E50"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="F13:F15"/>
+    <mergeCell ref="F26:F30"/>
+    <mergeCell ref="E31:E35"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
@@ -5149,78 +5204,20 @@
     <mergeCell ref="I51:I55"/>
     <mergeCell ref="F31:F35"/>
     <mergeCell ref="E36:E40"/>
-    <mergeCell ref="G26:G30"/>
-    <mergeCell ref="G10:G12"/>
-    <mergeCell ref="G13:G15"/>
-    <mergeCell ref="E26:E30"/>
-    <mergeCell ref="F36:F40"/>
-    <mergeCell ref="F46:F50"/>
-    <mergeCell ref="E51:E55"/>
-    <mergeCell ref="F51:F55"/>
-    <mergeCell ref="G51:G55"/>
-    <mergeCell ref="G31:G35"/>
-    <mergeCell ref="G36:G40"/>
-    <mergeCell ref="G41:G45"/>
-    <mergeCell ref="G46:G50"/>
-    <mergeCell ref="E41:E45"/>
-    <mergeCell ref="F41:F45"/>
-    <mergeCell ref="E46:E50"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="E13:E15"/>
-    <mergeCell ref="F13:F15"/>
-    <mergeCell ref="F26:F30"/>
-    <mergeCell ref="E31:E35"/>
-    <mergeCell ref="J10:J12"/>
-    <mergeCell ref="J13:J15"/>
-    <mergeCell ref="J26:J30"/>
-    <mergeCell ref="J31:J35"/>
-    <mergeCell ref="H10:H12"/>
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="H13:H15"/>
-    <mergeCell ref="I13:I15"/>
-    <mergeCell ref="H26:H30"/>
-    <mergeCell ref="I26:I30"/>
-    <mergeCell ref="H31:H35"/>
-    <mergeCell ref="M26:M30"/>
-    <mergeCell ref="N26:N30"/>
-    <mergeCell ref="M36:M40"/>
-    <mergeCell ref="N36:N40"/>
-    <mergeCell ref="M46:M50"/>
-    <mergeCell ref="N46:N50"/>
-    <mergeCell ref="J51:J55"/>
-    <mergeCell ref="L36:L40"/>
-    <mergeCell ref="K51:K55"/>
-    <mergeCell ref="L51:L55"/>
-    <mergeCell ref="J36:J40"/>
-    <mergeCell ref="J41:J45"/>
-    <mergeCell ref="J46:J50"/>
-    <mergeCell ref="K31:K35"/>
-    <mergeCell ref="L31:L35"/>
-    <mergeCell ref="M51:M55"/>
-    <mergeCell ref="N51:N55"/>
-    <mergeCell ref="M31:M35"/>
-    <mergeCell ref="N31:N35"/>
-    <mergeCell ref="N41:N45"/>
-    <mergeCell ref="M41:M45"/>
-    <mergeCell ref="U10:U12"/>
-    <mergeCell ref="U26:U30"/>
-    <mergeCell ref="U31:U35"/>
-    <mergeCell ref="U36:U40"/>
-    <mergeCell ref="U41:U45"/>
-    <mergeCell ref="R46:R50"/>
-    <mergeCell ref="U46:U50"/>
-    <mergeCell ref="O46:O50"/>
-    <mergeCell ref="O51:O55"/>
-    <mergeCell ref="P51:P55"/>
-    <mergeCell ref="Q51:Q55"/>
-    <mergeCell ref="O26:O30"/>
-    <mergeCell ref="O31:O35"/>
-    <mergeCell ref="O36:O40"/>
-    <mergeCell ref="O41:O45"/>
-    <mergeCell ref="S51:S55"/>
-    <mergeCell ref="T51:T55"/>
-    <mergeCell ref="U51:U55"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A6:D6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="P2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>